<commit_message>
feat: Add income management features including AddIncomeForm, IncomeList, and IncomePageOverview components
- Implemented AddIncomeForm for adding new income entries with emoji icon selection.
- Created IncomeList to display income sources with options to delete and download.
- Developed IncomePageOverview to visualize income trends using a bar chart.
- Added DeleteConfirmationModal for confirming deletion of income entries.
- Introduced Modal component for reusable modal functionality across the application.
- Created TransactionInfoCard for displaying individual income transactions with delete option.
</commit_message>
<xml_diff>
--- a/Backend/Incomes_details.xlsx
+++ b/Backend/Incomes_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,29 +415,84 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Freelancing</v>
+        <v>work</v>
       </c>
       <c r="B2">
-        <v>15000</v>
+        <v>3000</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-07-21</v>
+        <v>2025-08-01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Food Delivery</v>
+        <v>Prize</v>
       </c>
       <c r="B3">
-        <v>799</v>
+        <v>2000</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-07-21</v>
+        <v>2025-08-01</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Hackathon</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-07-29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Friend</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-07-28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Pocket money</v>
+      </c>
+      <c r="B6">
+        <v>5000</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-07-27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Interest</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-07-23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Gift</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-07-20</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>